<commit_message>
refactor table hs code
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">HS Code</t>
   </si>
@@ -32,18 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">PPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lartas_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lartas_border</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lartas_post_border</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lartas_export</t>
   </si>
   <si>
     <t xml:space="preserve">85353020</t>
@@ -134,8 +122,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,80 +151,72 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D86" activeCellId="0" sqref="D86"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Optimize by remove duplicate data on  hs codes list
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">HS Code</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">HS CODE</t>
   </si>
   <si>
     <t xml:space="preserve">BM</t>
@@ -34,7 +34,13 @@
     <t xml:space="preserve">PPH</t>
   </si>
   <si>
+    <t xml:space="preserve">PPH NON API</t>
+  </si>
+  <si>
     <t xml:space="preserve">85353020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">49111090</t>
@@ -151,10 +157,10 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -169,54 +175,164 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>